<commit_message>
Added New Stream Table Screenshot
</commit_message>
<xml_diff>
--- a/PFD_Stream_Table.xlsx
+++ b/PFD_Stream_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaoto\Desktop\School\CHEME\CHEME_485\Pontes_Ramos_Gao_Carpenter_485Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\College 19-20\Folder 485 - Process Design\Pontes_Ramos_Gao_Carpenter_485Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA9C033-49A8-4E15-8041-1F48C580095F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529F8984-45F4-40F3-88F4-B3EE9DE04559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6F586CE1-B146-4EEE-B671-C5DD4E8C1978}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{6F586CE1-B146-4EEE-B671-C5DD4E8C1978}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -452,21 +450,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A739691-ED40-42B6-BC62-183A5CF2EDDF}">
   <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="8.7265625" style="1"/>
-    <col min="18" max="18" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.17578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="8.703125" style="1"/>
+    <col min="18" max="18" width="9.8203125" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" customWidth="1"/>
+    <col min="20" max="20" width="8.8203125" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -531,12 +529,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.5">
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -601,7 +599,7 @@
         <v>234.4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -666,7 +664,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -731,7 +729,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -796,7 +794,7 @@
         <v>421.86399999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -861,7 +859,7 @@
         <v>7600</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -926,7 +924,7 @@
         <v>1375.57</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -991,7 +989,7 @@
         <v>-105.929</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1054,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1121,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1251,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1316,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1381,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>